<commit_message>
misc fixes for invoices like sort order, template change etc
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_invoice_Main_v3.xlsx
+++ b/application/controllers/excel-templates/partner_invoice_Main_v3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28016"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -71,10 +71,6 @@
 (Rs.)</t>
   </si>
   <si>
-    <t>Installation
-Charges</t>
-  </si>
-  <si>
     <t>Upcountry
 Charges</t>
   </si>
@@ -186,6 +182,9 @@
   </si>
   <si>
     <t>{meta:total_upcountry_charges}</t>
+  </si>
+  <si>
+    <t>Service Charges</t>
   </si>
 </sst>
 </file>
@@ -929,22 +928,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1" style="2" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="2" customWidth="1"/>
-    <col min="6" max="7" width="9.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -964,7 +964,7 @@
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -1073,7 +1073,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="11"/>
@@ -1082,13 +1082,13 @@
     <row r="11" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="11"/>
@@ -1097,13 +1097,13 @@
     <row r="12" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="11"/>
@@ -1116,7 +1116,7 @@
       <c r="D13" s="59"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="52"/>
       <c r="H13" s="34"/>
@@ -1153,7 +1153,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>11</v>
@@ -1162,40 +1162,40 @@
         <v>12</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="31" t="s">
         <v>14</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="E17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="53" t="s">
+      <c r="H17" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="35" t="s">
         <v>36</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1212,26 +1212,26 @@
     <row r="19" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I19" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="41">
         <v>5</v>
@@ -1239,7 +1239,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -1259,7 +1259,7 @@
     <row r="22" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="41">
         <v>14</v>
@@ -1270,13 +1270,13 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="41">
         <v>0.5</v>
@@ -1287,13 +1287,13 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="41">
         <v>0.5</v>
@@ -1304,7 +1304,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1321,26 +1321,26 @@
     <row r="26" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I26" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1349,7 +1349,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1366,10 +1366,10 @@
     <row r="29" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="56"/>
       <c r="E29" s="56"/>
@@ -1378,45 +1378,34 @@
       <c r="H29" s="56"/>
       <c r="I29" s="57"/>
     </row>
-    <row r="30" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="51"/>
+    </row>
+    <row r="31" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="51"/>
-    </row>
-    <row r="32" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
-      <c r="B32" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
+      <c r="B31" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="3">
-    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B31:I31"/>
     <mergeCell ref="C29:I29"/>
     <mergeCell ref="B12:D14"/>
   </mergeCells>

</xml_diff>